<commit_message>
4월 QQQ, SOXL 투자 추가
</commit_message>
<xml_diff>
--- a/심상범의 투자 일지.xlsx
+++ b/심상범의 투자 일지.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A\Documents\Investment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sangbeom\Documents\Investment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E61D621-A24C-4926-85F2-3F8297159CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251AA4E5-B066-4C83-B89C-6666514209D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1C587367-3A51-48E3-8FD5-9E60EF93E66E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{1C587367-3A51-48E3-8FD5-9E60EF93E66E}"/>
   </bookViews>
   <sheets>
     <sheet name="2025년" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>4월</t>
   </si>
@@ -149,6 +149,42 @@
   </si>
   <si>
     <t>총 평가 손익</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레버리지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOXL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레버리지 매수금액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레버리지 평가금액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레버리지 평가손익</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레버리지 수익률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목표</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>채권+금+달러</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고위험</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -158,8 +194,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="42" formatCode="_-&quot;₩&quot;* #,##0_-;\-&quot;₩&quot;* #,##0_-;_-&quot;₩&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.0%"/>
     <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="180" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -201,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -420,13 +456,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -484,31 +557,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -520,41 +581,47 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,6 +757,21 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:solidFill>
@@ -729,10 +811,10 @@
             </c:txPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="1"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
+            <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
             <c:extLst>
@@ -754,18 +836,21 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'2025년'!$B$26:$B$31</c15:sqref>
+                    <c15:sqref>'2025년'!$B$26:$B$32</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'2025년'!$B$30:$B$31</c:f>
+              <c:f>'2025년'!$B$30:$B$32</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>SCHD</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>QQQ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>레버리지</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -775,19 +860,22 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'2025년'!$C$26:$C$31</c15:sqref>
+                    <c15:sqref>'2025년'!$C$26:$C$32</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'2025년'!$C$30:$C$31</c:f>
+              <c:f>'2025년'!$C$30:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>_("₩"* #,##0_);_("₩"* \(#,##0\);_("₩"* "-"_);_(@_)</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0" formatCode="0.0%">
-                  <c:v>0.73783102277389245</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0" formatCode="0.00%">
+                  <c:v>0.55967923308366696</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="0.0%">
-                  <c:v>0.26216897722610749</c:v>
+                <c:pt idx="1" formatCode="0.00%">
+                  <c:v>0.41370642707668592</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00%">
+                  <c:v>2.661433983964713E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -802,8 +890,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1461,13 +1550,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1352550</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>203199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1812,37 +1901,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E3560C-3343-4AE5-82F6-2A10F2175E95}">
-  <dimension ref="B1:J34"/>
+  <dimension ref="B1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="5" width="19.625" customWidth="1"/>
-    <col min="7" max="7" width="14.125" customWidth="1"/>
-    <col min="8" max="10" width="19.625" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" customWidth="1"/>
+    <col min="3" max="5" width="19.59765625" customWidth="1"/>
+    <col min="7" max="7" width="16.19921875" customWidth="1"/>
+    <col min="8" max="10" width="19.59765625" customWidth="1"/>
+    <col min="12" max="12" width="16.19921875" customWidth="1"/>
+    <col min="13" max="15" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
+    <row r="1" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:15" ht="25.2" x14ac:dyDescent="0.4">
+      <c r="B2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-      <c r="G2" s="28" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="G2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="26"/>
+      <c r="L2" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="26"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B3" s="4"/>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -1857,8 +1954,14 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L3" s="4"/>
+      <c r="M3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1871,8 +1974,14 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="8"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1885,8 +1994,14 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="8"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
@@ -1899,8 +2014,14 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="8"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B7" s="6" t="s">
         <v>0</v>
       </c>
@@ -1915,12 +2036,21 @@
         <v>0</v>
       </c>
       <c r="H7" s="2">
-        <v>500080</v>
+        <f>500080+557700</f>
+        <v>1057780</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>69979</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="8"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
@@ -1933,8 +2063,14 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B9" s="6" t="s">
         <v>2</v>
       </c>
@@ -1947,8 +2083,14 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B10" s="6" t="s">
         <v>3</v>
       </c>
@@ -1961,8 +2103,14 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="8"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1975,8 +2123,14 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="8"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
@@ -1989,8 +2143,14 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="8"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
@@ -2003,8 +2163,14 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B14" s="6" t="s">
         <v>7</v>
       </c>
@@ -2017,8 +2183,14 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B15" s="6" t="s">
         <v>8</v>
       </c>
@@ -2031,8 +2203,14 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="8"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="8"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B16" s="6" t="s">
         <v>20</v>
       </c>
@@ -2050,42 +2228,59 @@
       </c>
       <c r="H16" s="2">
         <f>SUM(H4:H15)</f>
-        <v>500080</v>
+        <v>1057780</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="2">
+        <f>SUM(M4:M15)</f>
+        <v>69979</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="8"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="2">
-        <v>507615</v>
+        <v>507400</v>
       </c>
       <c r="D17" s="2">
-        <v>954544</v>
+        <v>956361</v>
       </c>
       <c r="E17" s="8"/>
       <c r="G17" s="6" t="s">
         <v>21</v>
       </c>
       <c r="H17" s="2">
-        <v>519540</v>
+        <v>1081990</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="2">
+        <v>69606</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="8"/>
+    </row>
+    <row r="18" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="13">
         <f>(C17/C16)-1</f>
-        <v>1.6795865633074891E-2</v>
+        <v>1.6365202411714019E-2</v>
       </c>
       <c r="D18" s="13">
         <f>(D17/D16)-1</f>
-        <v>-8.8445648840418389E-4</v>
+        <v>1.0173866351821381E-3</v>
       </c>
       <c r="E18" s="14"/>
       <c r="G18" s="7" t="s">
@@ -2093,167 +2288,254 @@
       </c>
       <c r="H18" s="11">
         <f>(H17/H16)-1</f>
-        <v>3.8913773796192652E-2</v>
+        <v>2.2887556958913979E-2</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="10"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" s="11">
+        <f>(M17/M16)-1</f>
+        <v>-5.3301704797152905E-3</v>
+      </c>
+      <c r="N18" s="9"/>
+      <c r="O18" s="10"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B19" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="35">
         <f>SUM(C16:E16)</f>
         <v>1454619</v>
       </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
       <c r="G19" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="37">
+      <c r="H19" s="33">
         <f>SUM(H16:J16)</f>
-        <v>500080</v>
-      </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="38"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+        <v>1057780</v>
+      </c>
+      <c r="I19" s="33"/>
+      <c r="J19" s="34"/>
+      <c r="L19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" s="33">
+        <f>SUM(M16:O16)</f>
+        <v>69979</v>
+      </c>
+      <c r="N19" s="33"/>
+      <c r="O19" s="34"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C20" s="38">
         <f>SUM(C17:E17)</f>
-        <v>1462159</v>
-      </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
+        <v>1463761</v>
+      </c>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40"/>
       <c r="G20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="39">
+      <c r="H20" s="31">
         <f>SUM(H17:J17)</f>
-        <v>519540</v>
-      </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="40"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+        <v>1081990</v>
+      </c>
+      <c r="I20" s="31"/>
+      <c r="J20" s="32"/>
+      <c r="L20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" s="31">
+        <f>SUM(M17:O17)</f>
+        <v>69606</v>
+      </c>
+      <c r="N20" s="31"/>
+      <c r="O20" s="32"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B21" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="38">
         <f>C20-C19</f>
-        <v>7540</v>
-      </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
+        <v>9142</v>
+      </c>
+      <c r="D21" s="39"/>
+      <c r="E21" s="40"/>
       <c r="G21" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="28">
         <f>H20-H19</f>
-        <v>19460</v>
-      </c>
-      <c r="I21" s="26"/>
-      <c r="J21" s="27"/>
-    </row>
-    <row r="22" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24210</v>
+      </c>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
+      <c r="L21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M21" s="28">
+        <f>M20-M19</f>
+        <v>-373</v>
+      </c>
+      <c r="N21" s="29"/>
+      <c r="O21" s="30"/>
+    </row>
+    <row r="22" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="35">
+      <c r="C22" s="20">
         <f>(C20/C19)-1</f>
-        <v>5.1834879098926478E-3</v>
-      </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36"/>
+        <v>6.2848072244348074E-3</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
       <c r="G22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="41">
+      <c r="H22" s="22">
         <f>(H20/H19)-1</f>
-        <v>3.8913773796192652E-2</v>
-      </c>
-      <c r="I22" s="41"/>
-      <c r="J22" s="42"/>
-    </row>
-    <row r="25" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+        <v>2.2887556958913979E-2</v>
+      </c>
+      <c r="I22" s="22"/>
+      <c r="J22" s="23"/>
+      <c r="L22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" s="22">
+        <f>(M20/M19)-1</f>
+        <v>-5.3301704797152905E-3</v>
+      </c>
+      <c r="N22" s="22"/>
+      <c r="O22" s="23"/>
+    </row>
+    <row r="25" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B26" s="17" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="16">
-        <f>SUM(C19,H19)</f>
-        <v>1954699</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+        <f>SUM(C19,H19,M19)</f>
+        <v>2582378</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B27" s="18" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="8">
-        <f>SUM(C20,H20)</f>
-        <v>1981699</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+        <f>SUM(C20,H20,M20)</f>
+        <v>2615357</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B28" s="18" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="8">
         <f>C27-C26</f>
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+        <v>32979</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B29" s="18" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="3">
         <f>(C27/C26)-1</f>
-        <v>1.3812868375130849E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+        <v>1.2770787235640846E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B30" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="3">
         <f>(C20/C27)</f>
-        <v>0.73783102277389245</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="20" t="s">
+        <v>0.55967923308366696</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B31" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="3">
         <f>(H20/C27)</f>
-        <v>0.26216897722610749</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="3" t="e">
-        <f>(C33/C32)-1</f>
-        <v>#DIV/0!</v>
+        <v>0.41370642707668592</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="19">
+        <f>(M20/C27)</f>
+        <v>2.661433983964713E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="M20:O20"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H22:J22"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="H21:J21"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>